<commit_message>
adding new tas cases
</commit_message>
<xml_diff>
--- a/Excels/Test data Selenium.xlsx
+++ b/Excels/Test data Selenium.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PageObjectModelSelenium\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C9913B-B312-4AD9-B22B-9F5B745D2D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7632EB3B-D2C4-4A77-9250-53E74F2F1780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4575" yWindow="3120" windowWidth="21600" windowHeight="11325" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="NewCarsTest" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +38,36 @@
   </si>
   <si>
     <t>Emad@40304030</t>
+  </si>
+  <si>
+    <t>carBrand</t>
+  </si>
+  <si>
+    <t>carTitle</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>BMW Cars</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>Hyundai Cars</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Toyota Cars</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>Honda Cars</t>
   </si>
 </sst>
 </file>
@@ -381,7 +412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -413,4 +444,59 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99A29617-2B76-4203-9A3A-8745EABA3954}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>